<commit_message>
nag add ng admin at cashier user (admin, admin123 / cashier, cashier123) user and pass ng bawat acc
</commit_message>
<xml_diff>
--- a/sales_report.xlsx
+++ b/sales_report.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,13 +472,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>45736.59125</v>
+        <v>45737.5359837963</v>
       </c>
     </row>
     <row r="3">
@@ -486,33 +486,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>140</v>
+        <v>35</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>45736.5912962963</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" t="n">
-        <v>75</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>45736.59137731481</v>
+        <v>45737.53607638889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added logistics dashboard in admin but still not working due to inputs
</commit_message>
<xml_diff>
--- a/sales_report.xlsx
+++ b/sales_report.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,16 +469,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
-        <v>120</v>
+        <v>225</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>45737.5359837963</v>
+        <v>45737.58293981481</v>
       </c>
     </row>
     <row r="3">
@@ -486,16 +486,118 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>56</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3360</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>45737.58299768518</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" t="n">
+        <v>280</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>45737.58461805555</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>8</v>
+      </c>
+      <c r="C5" t="n">
+        <v>56</v>
+      </c>
+      <c r="D5" t="n">
+        <v>280</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>45737.60230324074</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="C3" t="n">
+      <c r="B6" t="n">
         <v>1</v>
       </c>
-      <c r="D3" t="n">
-        <v>35</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>45737.53607638889</v>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" t="n">
+        <v>120</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>45737.61083333333</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>10</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" t="n">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>45737.62180555556</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>8</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>45737.97798611111</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>45738.01177083333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
another kaguluhan pero nag rurun lahat prob lang is ung log in its just plain and logis logistics_dashboard kulang functions need more editing dont forget to make it stand alone
</commit_message>
<xml_diff>
--- a/sales_report.xlsx
+++ b/sales_report.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,16 +469,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D2" t="n">
-        <v>225</v>
+        <v>1380</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>45737.58293981481</v>
+        <v>45738.05504629629</v>
       </c>
     </row>
     <row r="3">
@@ -486,16 +486,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>3360</v>
+        <v>140</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>45737.58299768518</v>
+        <v>45738.05511574074</v>
       </c>
     </row>
     <row r="4">
@@ -503,16 +503,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D4" t="n">
-        <v>280</v>
+        <v>900</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>45737.58461805555</v>
+        <v>45738.14853009259</v>
       </c>
     </row>
     <row r="5">
@@ -520,16 +520,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="D5" t="n">
-        <v>280</v>
+        <v>900</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>45737.60230324074</v>
+        <v>45738.14856481482</v>
       </c>
     </row>
     <row r="6">
@@ -546,7 +546,7 @@
         <v>120</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>45737.61083333333</v>
+        <v>45738.14869212963</v>
       </c>
     </row>
     <row r="7">
@@ -554,16 +554,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D7" t="n">
-        <v>10</v>
+        <v>900</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>45737.62180555556</v>
+        <v>45738.15077546296</v>
       </c>
     </row>
     <row r="8">
@@ -571,33 +571,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D8" t="n">
-        <v>5</v>
+        <v>1200</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>45737.97798611111</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="n">
-        <v>10</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" t="n">
-        <v>5</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>45738.01177083333</v>
+        <v>45738.15090277778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
next step is to try convert flask to django
</commit_message>
<xml_diff>
--- a/sales_report.xlsx
+++ b/sales_report.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,16 +469,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
+        <v>11</v>
+      </c>
+      <c r="C2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="n">
-        <v>23</v>
-      </c>
       <c r="D2" t="n">
-        <v>1380</v>
+        <v>1000000000000</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>45738.05504629629</v>
+        <v>45738.18789351852</v>
       </c>
     </row>
     <row r="3">
@@ -486,101 +486,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>140</v>
+        <v>180</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>45738.05511574074</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="n">
-        <v>15</v>
-      </c>
-      <c r="D4" t="n">
-        <v>900</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>45738.14853009259</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="n">
-        <v>15</v>
-      </c>
-      <c r="D5" t="n">
-        <v>900</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>45738.14856481482</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" t="n">
-        <v>120</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>45738.14869212963</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="n">
-        <v>15</v>
-      </c>
-      <c r="D7" t="n">
-        <v>900</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>45738.15077546296</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="n">
-        <v>20</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1200</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>45738.15090277778</v>
+        <v>45740.53111111111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>